<commit_message>
updated stock list to 200 NSE across files
</commit_message>
<xml_diff>
--- a/TradingBook.xlsx
+++ b/TradingBook.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="trade" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Adani Power</t>
   </si>
@@ -60,9 +61,6 @@
     <t>cipla</t>
   </si>
   <si>
-    <t>No clear signal</t>
-  </si>
-  <si>
     <t>godcon</t>
   </si>
   <si>
@@ -114,17 +112,47 @@
     <t>Commentary</t>
   </si>
   <si>
-    <t>30/10: First hour price gone to 5801, vwap gone to 5808</t>
-  </si>
-  <si>
-    <t>30/10: First hour price gone to 1561, vwap gone to 1566.87</t>
+    <t>position</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Paper Trade Date</t>
+  </si>
+  <si>
+    <t>Today EOD</t>
+  </si>
+  <si>
+    <t>2. bad day lost almost 3%, Q2 FY2026 results announced, which may caused the drop
+1. No clear signal</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>Always careful about near future events or result declaration</t>
+  </si>
+  <si>
+    <t>exit price</t>
+  </si>
+  <si>
+    <t>31/10: doesn't show too much promise, and in general news is also not for great uptrend, so will close position at 165.8 based on todays high</t>
+  </si>
+  <si>
+    <t>31/10:  due to average result dclared and change in managemt price went down, however putting stop loss at 1520 to avoid too much loss on this trade
+30/10: First hour price gone to 1561, vwap gone to 1566.87</t>
+  </si>
+  <si>
+    <t>31/10:price went down to 5800, should have bought at that level, in the end it is showing -CVD which is not sure if correct. Volume doubled, selling does happen. However looking at 1 day candle it is green umbrella at bottom and vwap also increased from 1st tick to last tick.. BUT VWAP is at 5818 whereas mkt price 5859.. so no clear direction
+30/10: First hour price gone to 5801, vwap gone to 5808</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,8 +172,16 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,8 +206,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -179,11 +221,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -196,6 +253,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,12 +544,13 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="81.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -503,7 +569,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3">
         <v>45960</v>
@@ -552,7 +618,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3">
         <v>45960</v>
@@ -579,9 +645,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>45960</v>
@@ -604,8 +670,8 @@
       <c r="I5">
         <v>75568</v>
       </c>
-      <c r="J5" t="s">
-        <v>11</v>
+      <c r="J5" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -613,7 +679,7 @@
         <v>45960</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>2585345</v>
@@ -639,7 +705,7 @@
         <v>45960</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>5573121</v>
@@ -657,7 +723,7 @@
         <v>65779</v>
       </c>
       <c r="J7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -665,7 +731,7 @@
         <v>45960</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>502785</v>
@@ -683,15 +749,15 @@
         <v>22000</v>
       </c>
       <c r="J8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>45960</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>2170625</v>
@@ -709,7 +775,7 @@
         <v>-9497</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -720,150 +786,252 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S4"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="16" max="16" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
+    <row r="1" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" s="3">
         <v>45960</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45961</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>4451329</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2">
-        <v>161.15</v>
+      <c r="F2" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="G2">
+        <v>162.57</v>
+      </c>
+      <c r="H2">
         <v>162.1</v>
       </c>
-      <c r="H2">
-        <f>I2/G2</f>
+      <c r="I2">
+        <f>J2/H2</f>
         <v>616.90314620604568</v>
       </c>
-      <c r="I2">
-        <f>0.1*S2</f>
+      <c r="J2">
+        <f>0.1*V2</f>
         <v>100000</v>
       </c>
-      <c r="J2">
-        <f>(F2-G2)*H2</f>
-        <v>-586.05798889573634</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
-      <c r="S2">
+      <c r="K2">
+        <f>(G2-H2)*I2</f>
+        <v>289.94447871684076</v>
+      </c>
+      <c r="L2">
+        <f>K2*100/(H2*I2)</f>
+        <v>0.28994447871684076</v>
+      </c>
+      <c r="M2">
+        <f>0.98*G2</f>
+        <v>159.3186</v>
+      </c>
+      <c r="N2">
+        <v>165.82</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2">
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" s="3">
         <v>45960</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45961</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>140033</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3">
-        <v>5807</v>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="G3">
+        <v>5859</v>
+      </c>
+      <c r="H3">
         <v>5855</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H4" si="0">I3/G3</f>
+      <c r="I3">
+        <f t="shared" ref="I3:I4" si="0">J3/H3</f>
         <v>17.079419299743808</v>
       </c>
-      <c r="I3">
-        <f>0.1*S2</f>
+      <c r="J3">
+        <f>0.1*V2</f>
         <v>100000</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J4" si="1">(F3-G3)*H3</f>
-        <v>-819.81212638770285</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="K3">
+        <f t="shared" ref="K3:K4" si="1">(G3-H3)*I3</f>
+        <v>68.317677198975232</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L4" si="2">K3*100/(H3*I3)</f>
+        <v>6.8317677198975232E-2</v>
+      </c>
+      <c r="O3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P3" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" s="3">
         <v>45960</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45961</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5">
+      <c r="E4" s="5">
         <v>177665</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4">
-        <v>1565.8</v>
+      <c r="F4" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="G4">
+        <v>1540.1</v>
+      </c>
+      <c r="H4">
         <v>1581.1</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <f t="shared" si="0"/>
         <v>63.247106444880153</v>
       </c>
-      <c r="I4">
-        <f>0.1*S2</f>
+      <c r="J4">
+        <f>0.1*V2</f>
         <v>100000</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f t="shared" si="1"/>
-        <v>-967.68072860666348</v>
-      </c>
-      <c r="M4" t="s">
-        <v>30</v>
+        <v>-2593.1313642400864</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>-2.5931313642400866</v>
+      </c>
+      <c r="M4">
+        <v>1520</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>165.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>